<commit_message>
attempt to use an app form for enrollment.
- medic/config-itech#5
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -5,39 +5,45 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-6\zazic-scale-up\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-21\zazic-scale-up\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4289F53A-F71A-4A25-B4F1-5F01D7807B81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9F221-2849-430F-943C-D54A29A06695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgs0B2FIV/URLPJ5dImFvMgLsT6sg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjVZjTvRohpHUR2PhEjUV9EebBD5A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
   <si>
     <t>list_name</t>
   </si>
   <si>
+    <t>form_title</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
-    <t>form_title</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
     <t>path</t>
   </si>
   <si>
+    <t>Enroll New Person</t>
+  </si>
+  <si>
     <t>relevant</t>
   </si>
   <si>
@@ -89,18 +98,21 @@
     <t>required</t>
   </si>
   <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>enroll</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
+  </si>
+  <si>
     <t>hint</t>
   </si>
   <si>
     <t>default</t>
   </si>
   <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
     <t>calculation</t>
   </si>
   <si>
@@ -110,15 +122,15 @@
     <t>instance::db-doc-ref</t>
   </si>
   <si>
-    <t>Enroll New Person</t>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
   <si>
     <t>begin group</t>
   </si>
   <si>
-    <t>enroll</t>
-  </si>
-  <si>
     <t>inputs</t>
   </si>
   <si>
@@ -131,12 +143,6 @@
     <t>field-list</t>
   </si>
   <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -179,214 +185,187 @@
     <t>Select a person from list</t>
   </si>
   <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
     <t>end group</t>
   </si>
   <si>
     <t>calculate</t>
   </si>
   <si>
+    <t>patient_name</t>
+  </si>
+  <si>
+    <t>patient_uuid</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>${person}</t>
+  </si>
+  <si>
+    <t>Patient Phone</t>
+  </si>
+  <si>
+    <t>../person/phone</t>
+  </si>
+  <si>
+    <t>Language preference</t>
+  </si>
+  <si>
+    <t>../person/language_preference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>../../../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>../../../../inputs/contact/parent/_id</t>
+  </si>
+  <si>
+    <t>Person Type</t>
+  </si>
+  <si>
+    <t>"person"</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>../../inputs/contact/parent/_id</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>../../inputs/contact/name</t>
+  </si>
+  <si>
+    <t>n_parent_id</t>
+  </si>
+  <si>
+    <t>VMMC Client Name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Client Mobile phone number</t>
+  </si>
+  <si>
+    <t>regex(., '^\+?\d{3,15}$')</t>
+  </si>
+  <si>
+    <t>alternative_phone</t>
+  </si>
+  <si>
+    <t>Alternative/Next of Kin's Mobile Number</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>select_one language_preference</t>
+  </si>
+  <si>
+    <t>What is this client’s language of preference for the texts?</t>
+  </si>
+  <si>
+    <t>enrollment_location</t>
+  </si>
+  <si>
+    <t>Specify Enrollment Location</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
+  </si>
+  <si>
+    <t>Please type in name characters e.g letters and space.</t>
+  </si>
+  <si>
+    <t>vmmc_no</t>
+  </si>
+  <si>
+    <t>VMMC Client Number</t>
+  </si>
+  <si>
+    <t>regex(., '^[0-9]{5,9}$')</t>
+  </si>
+  <si>
+    <t>Must be 5 – 9 numeric digits</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>age_years</t>
+  </si>
+  <si>
+    <t>VMMC Client Age in Years</t>
+  </si>
+  <si>
+    <t>(.) &gt;= 18 and (.) &lt;= 75</t>
+  </si>
+  <si>
+    <t>Only 18 - 75 yrs old men can enroll.</t>
+  </si>
+  <si>
+    <t>enrollment_nurse</t>
+  </si>
+  <si>
+    <t>Name of enrollment nurse</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>enrollment_date</t>
+  </si>
+  <si>
+    <t>Enrollment Date</t>
+  </si>
+  <si>
     <t>place_id</t>
   </si>
   <si>
-    <t>NO_LABEL</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>../inputs/contact/_id</t>
   </si>
   <si>
-    <t>patient_uuid</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>${person}</t>
-  </si>
-  <si>
-    <t>patient_id</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>../person/phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true </t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>../../../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t>../../inputs/contact/parent/_id != ''</t>
-  </si>
-  <si>
-    <t>../../../inputs/contact/parent/_id</t>
-  </si>
-  <si>
-    <t>Person Type</t>
-  </si>
-  <si>
-    <t>"person"</t>
-  </si>
-  <si>
-    <t>VMMC Client Name</t>
-  </si>
-  <si>
-    <t>select_one facilities</t>
-  </si>
-  <si>
-    <t>enrollment_facility</t>
-  </si>
-  <si>
-    <t>VMMC Enrollment Facility</t>
-  </si>
-  <si>
-    <t>enrollment_location</t>
-  </si>
-  <si>
-    <t>Specify Enrollment Location</t>
-  </si>
-  <si>
-    <t>${enrollment_facility} = 'other'</t>
-  </si>
-  <si>
-    <t>vmmc_no</t>
-  </si>
-  <si>
-    <t>VMMC Client Number</t>
-  </si>
-  <si>
-    <t>regex(., '[0-9]{5,9}')</t>
-  </si>
-  <si>
-    <t>Must be 5 – 9 numeric digits</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>age_years</t>
-  </si>
-  <si>
-    <t>VMMC Client Age in Years</t>
-  </si>
-  <si>
-    <t>(.) &gt;= 18 and (.) &lt;= 75</t>
-  </si>
-  <si>
-    <t>Only over 18 yrs men can enroll.</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>enrollment_date</t>
-  </si>
-  <si>
-    <t>Enrollment Date</t>
-  </si>
-  <si>
-    <t>decimal-date-time(.) = floor(decimal-date-time(today()))</t>
-  </si>
-  <si>
-    <t>Only today's date is allowed</t>
-  </si>
-  <si>
-    <t>Client Mobile phone number</t>
-  </si>
-  <si>
-    <t>regex(., '^\+?\d{3,15}$')</t>
-  </si>
-  <si>
-    <t>alternative_phone</t>
-  </si>
-  <si>
-    <t>Alternative/Next of Kin's Mobile Number</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>select_one language_preference</t>
-  </si>
-  <si>
-    <t>What is this client’s language of preference for the texts?</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>enrollment_nurse</t>
-  </si>
-  <si>
-    <t>Name of enrollment nurse</t>
-  </si>
-  <si>
-    <t>Chitungwiza-Seke North clinic</t>
-  </si>
-  <si>
-    <t>Chitungwiza-Seke South clinic</t>
-  </si>
-  <si>
-    <t>Chitungwiza-City Med hospital</t>
-  </si>
-  <si>
-    <t>Chitungwiza-Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>Chitungwiza-Chitungwiza Central Hospital</t>
-  </si>
-  <si>
-    <t>Chegutu- Norton hospital</t>
-  </si>
-  <si>
-    <t>Chegutu- District Hospital</t>
-  </si>
-  <si>
-    <t>Chegutu- Monera clinic (Norton Outreach)</t>
-  </si>
-  <si>
-    <t>Marondera- Marondera District Hospital</t>
-  </si>
-  <si>
-    <t>Marondera- Mahusekwa Hospital</t>
-  </si>
-  <si>
-    <t>csnc</t>
-  </si>
-  <si>
-    <t>cssc</t>
-  </si>
-  <si>
-    <t>ccmh</t>
-  </si>
-  <si>
-    <t>czc</t>
-  </si>
-  <si>
-    <t>ccch</t>
-  </si>
-  <si>
-    <t>cnh</t>
-  </si>
-  <si>
-    <t>cdh</t>
-  </si>
-  <si>
-    <t>cmc</t>
-  </si>
-  <si>
-    <t>mmdh</t>
-  </si>
-  <si>
-    <t>mmh</t>
+    <t>../person/name</t>
+  </si>
+  <si>
+    <t>decimal-date-time(.) &lt;= floor(decimal-date-time(today()))</t>
+  </si>
+  <si>
+    <t>Date cannot be in the future</t>
+  </si>
+  <si>
+    <t>Parent id: ${parent_id}, Name: ${contact_name}</t>
   </si>
 </sst>
 </file>
@@ -396,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -414,23 +393,6 @@
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -438,43 +400,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF843C0B"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF833C0C"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -522,60 +476,46 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,117 +731,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="13.25" customWidth="1"/>
-    <col min="10" max="16" width="13.5" customWidth="1"/>
-    <col min="17" max="26" width="10" customWidth="1"/>
+    <col min="1" max="1" width="28.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="7" customWidth="1"/>
+    <col min="6" max="8" width="13.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.25" style="7" customWidth="1"/>
+    <col min="10" max="12" width="13.5" style="7" customWidth="1"/>
+    <col min="13" max="13" width="17.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="13.5" style="7" customWidth="1"/>
+    <col min="17" max="26" width="10" style="7" customWidth="1"/>
+    <col min="27" max="16384" width="11.25" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="J1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="L1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -910,106 +838,58 @@
       <c r="B3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -1018,994 +898,724 @@
       <c r="B6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="13"/>
       <c r="E6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
+      <c r="A8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A9" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="19" t="s">
+      <c r="C9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A11" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A12" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
+      <c r="A12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
+      <c r="A13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
+      <c r="A14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="19" t="s">
+      <c r="A15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
+      <c r="K15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="A16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
+      <c r="K16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="C17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
+      <c r="A18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A19" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A20" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="A20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A21" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="21" t="s">
+      <c r="A21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="24" t="s">
+      <c r="C21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
+      <c r="A22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
+      <c r="A23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
+      <c r="A24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
+      <c r="A25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
+      <c r="A26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
+      <c r="A27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
+      <c r="A28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+    </row>
+    <row r="30" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+    </row>
+    <row r="31" spans="1:26" ht="14.25">
+      <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+    </row>
+    <row r="32" spans="1:26" s="14" customFormat="1" ht="15.75">
+      <c r="A32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+    </row>
+    <row r="33" spans="1:26" s="14" customFormat="1" ht="15.75">
+      <c r="A33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="H33" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+    </row>
+    <row r="34" spans="1:26" ht="14.25">
+      <c r="A34" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
+      <c r="B34" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75">
-      <c r="A30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="3" t="s">
+    <row r="35" spans="1:26" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+    </row>
+    <row r="36" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+    </row>
+    <row r="37" spans="1:26" ht="14.25">
+      <c r="A37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+    </row>
+    <row r="38" spans="1:26" ht="14.25">
+      <c r="A38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
+      <c r="C38" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75">
-      <c r="A31" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="29" t="s">
+    <row r="39" spans="1:26" s="14" customFormat="1" ht="15.75">
+      <c r="A39" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
+      <c r="C39" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="12"/>
+      <c r="Z39" s="12"/>
     </row>
-    <row r="32" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
+    <row r="40" spans="1:26" ht="15" customHeight="1">
+      <c r="A40" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="38" ht="12.75" customHeight="1"/>
-    <row r="39" ht="12.75" customHeight="1"/>
-    <row r="40" ht="12.75" customHeight="1"/>
-    <row r="41" ht="12.75" customHeight="1"/>
-    <row r="42" ht="12.75" customHeight="1"/>
-    <row r="43" ht="12.75" customHeight="1"/>
-    <row r="44" ht="12.75" customHeight="1"/>
-    <row r="45" ht="12.75" customHeight="1"/>
-    <row r="46" ht="12.75" customHeight="1"/>
-    <row r="47" ht="12.75" customHeight="1"/>
-    <row r="48" ht="12.75" customHeight="1"/>
+    <row r="42" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="43" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="44" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="45" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="46" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="47" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="48" spans="1:26" ht="12.75" customHeight="1"/>
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1"/>
     <row r="51" ht="12.75" customHeight="1"/>
@@ -2190,10 +1800,10 @@
     <row r="230" ht="12.75" customHeight="1"/>
     <row r="231" ht="12.75" customHeight="1"/>
     <row r="232" ht="12.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="233" ht="12.75" customHeight="1"/>
+    <row r="234" ht="12.75" customHeight="1"/>
+    <row r="235" ht="12.75" customHeight="1"/>
+    <row r="236" ht="12.75" customHeight="1"/>
     <row r="237" ht="15.75" customHeight="1"/>
     <row r="238" ht="15.75" customHeight="1"/>
     <row r="239" ht="15.75" customHeight="1"/>
@@ -2965,9 +2575,13 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2975,16 +2589,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="35.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
     <col min="4" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
@@ -3027,127 +2641,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -4123,7 +3634,7 @@
     <row r="989" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4145,7 +3656,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>13</v>
@@ -4171,31 +3682,31 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43900</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="10">
-        <v>43900</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
#9 Updated the facilities list in the enrollment form
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-6\zazic-scale-up\forms\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4289F53A-F71A-4A25-B4F1-5F01D7807B81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgs0B2FIV/URLPJ5dImFvMgLsT6sg=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="120">
   <si>
     <t>list_name</t>
   </si>
@@ -318,88 +327,154 @@
   </si>
   <si>
     <t>Name of enrollment nurse</t>
+  </si>
+  <si>
+    <t>Chitungwiza-Seke North clinic</t>
+  </si>
+  <si>
+    <t>Chitungwiza-Seke South clinic</t>
+  </si>
+  <si>
+    <t>Chitungwiza-City Med hospital</t>
+  </si>
+  <si>
+    <t>Chitungwiza-Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>Chitungwiza-Chitungwiza Central Hospital</t>
+  </si>
+  <si>
+    <t>Chegutu- Norton hospital</t>
+  </si>
+  <si>
+    <t>Chegutu- District Hospital</t>
+  </si>
+  <si>
+    <t>Chegutu- Monera clinic (Norton Outreach)</t>
+  </si>
+  <si>
+    <t>Marondera- Marondera District Hospital</t>
+  </si>
+  <si>
+    <t>Marondera- Mahusekwa Hospital</t>
+  </si>
+  <si>
+    <t>csnc</t>
+  </si>
+  <si>
+    <t>cssc</t>
+  </si>
+  <si>
+    <t>ccmh</t>
+  </si>
+  <si>
+    <t>czc</t>
+  </si>
+  <si>
+    <t>ccch</t>
+  </si>
+  <si>
+    <t>cnh</t>
+  </si>
+  <si>
+    <t>cdh</t>
+  </si>
+  <si>
+    <t>cmc</t>
+  </si>
+  <si>
+    <t>mmdh</t>
+  </si>
+  <si>
+    <t>mmh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF843C0B"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -407,7 +482,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -417,7 +492,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
@@ -431,131 +512,89 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -745,34 +784,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.11"/>
-    <col customWidth="1" min="2" max="2" width="18.44"/>
-    <col customWidth="1" min="3" max="3" width="57.0"/>
-    <col customWidth="1" min="4" max="4" width="11.33"/>
-    <col customWidth="1" min="5" max="5" width="11.78"/>
-    <col customWidth="1" min="6" max="8" width="13.44"/>
-    <col customWidth="1" min="9" max="9" width="13.22"/>
-    <col customWidth="1" min="10" max="16" width="13.44"/>
-    <col customWidth="1" min="17" max="26" width="10.0"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="57" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="16" width="13.5" customWidth="1"/>
+    <col min="17" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -826,7 +865,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
@@ -864,7 +903,7 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -902,7 +941,7 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -938,7 +977,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -972,7 +1011,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
+    <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>45</v>
       </c>
@@ -1010,7 +1049,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
@@ -1040,7 +1079,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>50</v>
       </c>
@@ -1070,7 +1109,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>51</v>
       </c>
@@ -1108,7 +1147,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1">
       <c r="A10" s="20" t="s">
         <v>51</v>
       </c>
@@ -1147,7 +1186,7 @@
       <c r="Y10" s="25"/>
       <c r="Z10" s="25"/>
     </row>
-    <row r="11" ht="12.75" customHeight="1">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>51</v>
       </c>
@@ -1186,7 +1225,7 @@
       <c r="Y11" s="23"/>
       <c r="Z11" s="23"/>
     </row>
-    <row r="12" ht="12.75" customHeight="1">
+    <row r="12" spans="1:26" ht="12.75" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>51</v>
       </c>
@@ -1223,7 +1262,7 @@
       <c r="Y12" s="23"/>
       <c r="Z12" s="23"/>
     </row>
-    <row r="13" ht="12.75" customHeight="1">
+    <row r="13" spans="1:26" ht="12.75" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>28</v>
       </c>
@@ -1261,7 +1300,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
+    <row r="14" spans="1:26" ht="12.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>28</v>
       </c>
@@ -1297,7 +1336,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
+    <row r="15" spans="1:26" ht="12.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>51</v>
       </c>
@@ -1335,7 +1374,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
+    <row r="16" spans="1:26" ht="12.75" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>28</v>
       </c>
@@ -1373,7 +1412,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
+    <row r="17" spans="1:26" ht="12.75" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>51</v>
       </c>
@@ -1411,7 +1450,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" ht="12.75" customHeight="1">
+    <row r="18" spans="1:26" ht="12.75" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>50</v>
       </c>
@@ -1441,7 +1480,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1">
+    <row r="19" spans="1:26" ht="12.75" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>50</v>
       </c>
@@ -1471,7 +1510,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
+    <row r="20" spans="1:26" ht="12.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>51</v>
       </c>
@@ -1509,7 +1548,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" ht="12.75" customHeight="1">
+    <row r="21" spans="1:26" ht="12.75" customHeight="1">
       <c r="A21" s="21" t="s">
         <v>51</v>
       </c>
@@ -1548,7 +1587,7 @@
       <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
     </row>
-    <row r="22" ht="12.75" customHeight="1">
+    <row r="22" spans="1:26" ht="12.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1584,7 +1623,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" ht="12.75" customHeight="1">
+    <row r="23" spans="1:26" ht="12.75" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>70</v>
       </c>
@@ -1620,7 +1659,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" ht="12.75" customHeight="1">
+    <row r="24" spans="1:26" ht="12.75" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -1658,7 +1697,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" ht="12.75" customHeight="1">
+    <row r="25" spans="1:26" ht="12.75" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1737,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" ht="12.75" customHeight="1">
+    <row r="26" spans="1:26" ht="12.75" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>80</v>
       </c>
@@ -1738,7 +1777,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" ht="12.75" customHeight="1">
+    <row r="27" spans="1:26" ht="12.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -1778,7 +1817,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" ht="12.75" customHeight="1">
+    <row r="28" spans="1:26" ht="12.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -1816,7 +1855,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
+    <row r="29" spans="1:26" ht="12.75" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1854,7 +1893,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" ht="15.75">
       <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
@@ -1890,7 +1929,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" ht="15.75">
       <c r="A31" s="3" t="s">
         <v>97</v>
       </c>
@@ -1926,7 +1965,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" ht="12.75" customHeight="1">
+    <row r="32" spans="1:26" ht="12.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>50</v>
       </c>
@@ -2927,34 +2966,30 @@
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.67"/>
-    <col customWidth="1" min="2" max="2" width="13.44"/>
-    <col customWidth="1" min="3" max="3" width="17.67"/>
-    <col customWidth="1" min="4" max="6" width="13.44"/>
-    <col customWidth="1" min="7" max="26" width="8.56"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="35.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2965,12 +3000,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2981,7 +3016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2992,24 +3027,127 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3984,32 +4122,28 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.67"/>
-    <col customWidth="1" min="2" max="2" width="53.33"/>
-    <col customWidth="1" min="3" max="3" width="40.0"/>
-    <col customWidth="1" min="4" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="15" width="13.44"/>
-    <col customWidth="1" min="16" max="26" width="8.56"/>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="53.375" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
+    <row r="1" spans="1:15" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4036,7 +4170,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -4044,7 +4178,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="10">
-        <v>43900.0</v>
+        <v>43900</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>34</v>
@@ -5044,9 +5178,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zazic-scale-up: update scheduled messages and add no contact task
- #48
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mj+hzUDfBjeNr5LSuO88yzzyyymRg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjXFJf4g09O0S+55HUHwMMEIA8zcg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Source ID</t>
+  </si>
+  <si>
+    <t>is_task</t>
+  </si>
+  <si>
+    <t>Is Task</t>
   </si>
   <si>
     <t>contact</t>
@@ -950,22 +956,24 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
+      <c r="A5" s="5" t="s">
+        <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -985,26 +993,20 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -1025,22 +1027,26 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -1064,7 +1070,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>35</v>
@@ -1073,7 +1079,7 @@
       <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>36</v>
@@ -1106,7 +1112,9 @@
         <v>37</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1131,13 +1139,13 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1165,10 +1173,14 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1195,7 +1207,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1225,7 +1237,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1255,14 +1267,10 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1270,9 +1278,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1291,18 +1297,16 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1312,9 +1316,7 @@
         <v>44</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1331,13 +1333,13 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
@@ -1349,10 +1351,12 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -1369,16 +1373,18 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>34</v>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1405,13 +1411,13 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1421,7 +1427,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1440,9 +1446,15 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1450,7 +1462,9 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -1468,28 +1482,18 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1510,14 +1514,14 @@
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1525,7 +1529,9 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1543,13 +1549,13 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
@@ -1560,9 +1566,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -1581,24 +1585,26 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -1617,26 +1623,24 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -1655,18 +1659,26 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -1685,7 +1697,7 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1715,26 +1727,18 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1751,65 +1755,67 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28">
-      <c r="A28" s="6" t="s">
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -1824,32 +1830,26 @@
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>18</v>
+      <c r="A30" s="7" t="s">
+        <v>63</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>66</v>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>33</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -1870,42 +1870,44 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="G31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
@@ -1914,25 +1916,23 @@
         <v>18</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="4"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1953,111 +1953,111 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="H33" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="10" t="s">
-        <v>18</v>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>79</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>34</v>
+      <c r="B34" s="3" t="s">
+        <v>80</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="10" t="s">
+      <c r="H34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="J34" s="9"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="7"/>
-      <c r="X34" s="7"/>
-      <c r="Y34" s="7"/>
-      <c r="Z34" s="7"/>
-    </row>
-    <row r="35">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+    </row>
+    <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="7"/>
@@ -2078,50 +2078,62 @@
       <c r="Z35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5" t="s">
-        <v>31</v>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>69</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
-    </row>
-    <row r="37" ht="15.0" customHeight="1">
+      <c r="G36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="9"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+    </row>
+    <row r="37">
       <c r="A37" s="4" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="F37" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -2136,15 +2148,17 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="4"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+    </row>
+    <row r="38" ht="15.0" customHeight="1">
+      <c r="A38" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2171,7 +2185,7 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
+    <row r="39">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -7631,7 +7645,7 @@
       <c r="Y233" s="4"/>
       <c r="Z233" s="4"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" ht="12.75" customHeight="1">
       <c r="A234" s="4"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
@@ -29330,6 +29344,34 @@
       <c r="X1008" s="4"/>
       <c r="Y1008" s="4"/>
       <c r="Z1008" s="4"/>
+    </row>
+    <row r="1009" ht="15.75" customHeight="1">
+      <c r="A1009" s="4"/>
+      <c r="B1009" s="4"/>
+      <c r="C1009" s="4"/>
+      <c r="D1009" s="4"/>
+      <c r="E1009" s="4"/>
+      <c r="F1009" s="4"/>
+      <c r="G1009" s="4"/>
+      <c r="H1009" s="4"/>
+      <c r="I1009" s="4"/>
+      <c r="J1009" s="4"/>
+      <c r="K1009" s="4"/>
+      <c r="L1009" s="4"/>
+      <c r="M1009" s="4"/>
+      <c r="N1009" s="4"/>
+      <c r="O1009" s="4"/>
+      <c r="P1009" s="4"/>
+      <c r="Q1009" s="4"/>
+      <c r="R1009" s="4"/>
+      <c r="S1009" s="4"/>
+      <c r="T1009" s="4"/>
+      <c r="U1009" s="4"/>
+      <c r="V1009" s="4"/>
+      <c r="W1009" s="4"/>
+      <c r="X1009" s="4"/>
+      <c r="Y1009" s="4"/>
+      <c r="Z1009" s="4"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -29361,7 +29403,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -29423,13 +29465,13 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -29457,13 +29499,13 @@
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -29519,13 +29561,13 @@
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -29553,13 +29595,13 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -29587,13 +29629,13 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -29621,13 +29663,13 @@
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -29655,13 +29697,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -29689,13 +29731,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -29723,13 +29765,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -29757,13 +29799,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -29791,13 +29833,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -29825,13 +29867,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -29859,13 +29901,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -57163,19 +57205,19 @@
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
@@ -57190,19 +57232,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C2" s="23">
         <v>43900.0</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>

</xml_diff>

<commit_message>
Zazic scale up adding sms translations (#222)
* outbound push for rapidPro added in the app_settings.json

* ndebele language option added to 2Wt

* files cleaned up

* files cleaned up

* resolving merging conflicts

* resolving merging conflicts

* resolving merging conflicts
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amatsii-dev\medic\config-itech\zazic-scale-up\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414683DD-3484-674D-B7F8-D1B7BEEFBD67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4E03FB-D502-4665-A3FB-072D7C800DDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="198">
   <si>
     <t>type</t>
   </si>
@@ -617,6 +617,12 @@
   <si>
     <t>44. Other</t>
   </si>
+  <si>
+    <t>ndebele</t>
+  </si>
+  <si>
+    <t>Ndebele</t>
+  </si>
 </sst>
 </file>
 
@@ -963,21 +969,21 @@
       <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="43.1640625" customWidth="1"/>
-    <col min="8" max="8" width="50.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="43.125" customWidth="1"/>
+    <col min="8" max="8" width="50.125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
     <col min="10" max="10" width="13.5" customWidth="1"/>
     <col min="11" max="11" width="25.5" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.375" customWidth="1"/>
     <col min="14" max="16" width="13.5" customWidth="1"/>
     <col min="17" max="26" width="10" customWidth="1"/>
   </cols>
@@ -1986,7 +1992,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="16">
+    <row r="29" spans="1:26" ht="15.75">
       <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
@@ -2026,7 +2032,7 @@
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
     </row>
-    <row r="30" spans="1:26" ht="16">
+    <row r="30" spans="1:26" ht="15.75">
       <c r="A30" s="7" t="s">
         <v>63</v>
       </c>
@@ -2064,7 +2070,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="16">
+    <row r="31" spans="1:26" ht="15.75">
       <c r="A31" s="10" t="s">
         <v>18</v>
       </c>
@@ -2106,7 +2112,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" ht="16">
+    <row r="32" spans="1:26" ht="15.75">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -2146,7 +2152,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" ht="16">
+    <row r="33" spans="1:26" ht="15.75">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -2188,7 +2194,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" ht="16">
+    <row r="34" spans="1:26" ht="15.75">
       <c r="A34" s="3" t="s">
         <v>79</v>
       </c>
@@ -2272,7 +2278,7 @@
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
     </row>
-    <row r="36" spans="1:26" ht="16">
+    <row r="36" spans="1:26" ht="15.75">
       <c r="A36" s="10" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2320,7 @@
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="1:26" ht="16">
+    <row r="37" spans="1:26" ht="15.75">
       <c r="A37" s="4" t="s">
         <v>90</v>
       </c>
@@ -2380,7 +2386,7 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
     </row>
-    <row r="39" spans="1:26" ht="16">
+    <row r="39" spans="1:26" ht="15.75">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -29576,23 +29582,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
     <col min="4" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16">
+    <row r="1" spans="1:26" ht="15.75">
       <c r="A1" s="14" t="s">
         <v>92</v>
       </c>
@@ -29626,7 +29632,7 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" ht="16">
+    <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -29654,7 +29660,7 @@
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
     </row>
-    <row r="3" spans="1:26" ht="16">
+    <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="14" t="s">
         <v>52</v>
       </c>
@@ -29688,7 +29694,7 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
     </row>
-    <row r="4" spans="1:26" ht="16">
+    <row r="4" spans="1:26" ht="15.75">
       <c r="A4" s="14" t="s">
         <v>52</v>
       </c>
@@ -29722,10 +29728,16 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="16">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+    <row r="5" spans="1:26" ht="15.75">
+      <c r="A5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>197</v>
+      </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -29750,49 +29762,43 @@
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="16">
-      <c r="A6" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>110</v>
-      </c>
+    <row r="6" spans="1:26" ht="15.75">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-    </row>
-    <row r="7" spans="1:26" ht="16">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
@@ -29818,15 +29824,15 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" ht="16">
+    <row r="8" spans="1:26" ht="15.75">
       <c r="A8" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
@@ -29852,15 +29858,15 @@
       <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" ht="16">
+    <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
@@ -29886,15 +29892,15 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
@@ -29925,10 +29931,10 @@
         <v>97</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
@@ -29959,10 +29965,10 @@
         <v>97</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
@@ -29989,14 +29995,14 @@
       <c r="Z12" s="16"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>123</v>
+      <c r="B13" s="21" t="s">
+        <v>121</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>124</v>
+      <c r="C13" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
@@ -30027,10 +30033,10 @@
         <v>97</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
@@ -30061,10 +30067,10 @@
         <v>97</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
@@ -30095,44 +30101,44 @@
         <v>97</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -30163,10 +30169,10 @@
         <v>97</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -30192,27 +30198,49 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" ht="15" customHeight="1">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1">
       <c r="A20" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D20" s="15"/>
     </row>
@@ -30221,10 +30249,10 @@
         <v>97</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21" s="15"/>
     </row>
@@ -30233,10 +30261,10 @@
         <v>97</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D22" s="15"/>
     </row>
@@ -30245,10 +30273,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D23" s="15"/>
     </row>
@@ -30257,10 +30285,10 @@
         <v>97</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D24" s="15"/>
     </row>
@@ -30269,55 +30297,34 @@
         <v>97</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -30347,17 +30354,16 @@
         <v>97</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
@@ -30377,14 +30383,14 @@
       <c r="Z28" s="15"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>155</v>
+      <c r="B29" s="15" t="s">
+        <v>153</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>156</v>
+      <c r="C29" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -30415,10 +30421,10 @@
         <v>97</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -30449,10 +30455,10 @@
         <v>97</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -30483,10 +30489,10 @@
         <v>97</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
@@ -30517,16 +30523,17 @@
         <v>97</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
@@ -30550,10 +30557,10 @@
         <v>97</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -30583,10 +30590,10 @@
         <v>97</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -30616,10 +30623,10 @@
         <v>97</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
@@ -30649,10 +30656,10 @@
         <v>97</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
@@ -30682,10 +30689,10 @@
         <v>97</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
@@ -30715,10 +30722,10 @@
         <v>97</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
@@ -30748,10 +30755,10 @@
         <v>97</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -30781,10 +30788,10 @@
         <v>97</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -30814,10 +30821,10 @@
         <v>97</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
@@ -30847,10 +30854,10 @@
         <v>97</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -30880,17 +30887,16 @@
         <v>97</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -30914,10 +30920,10 @@
         <v>97</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
@@ -30948,10 +30954,10 @@
         <v>97</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
@@ -30982,10 +30988,10 @@
         <v>97</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -31016,10 +31022,10 @@
         <v>97</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
@@ -31046,14 +31052,14 @@
       <c r="Z48" s="15"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>98</v>
+      <c r="B49" s="14" t="s">
+        <v>193</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>195</v>
+      <c r="C49" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
@@ -31080,9 +31086,15 @@
       <c r="Z49" s="15"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
+      <c r="A50" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>195</v>
+      </c>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
@@ -31116,6 +31128,7 @@
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
@@ -31143,7 +31156,6 @@
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
@@ -56447,6 +56459,10 @@
       <c r="Z955" s="15"/>
     </row>
     <row r="956" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A956" s="15"/>
+      <c r="B956" s="15"/>
+      <c r="C956" s="15"/>
+      <c r="D956" s="15"/>
       <c r="E956" s="15"/>
       <c r="F956" s="15"/>
       <c r="G956" s="15"/>
@@ -57262,6 +57278,30 @@
       <c r="Y989" s="15"/>
       <c r="Z989" s="15"/>
     </row>
+    <row r="990" spans="5:26" ht="15.75" customHeight="1">
+      <c r="E990" s="15"/>
+      <c r="F990" s="15"/>
+      <c r="G990" s="15"/>
+      <c r="H990" s="15"/>
+      <c r="I990" s="15"/>
+      <c r="J990" s="15"/>
+      <c r="K990" s="15"/>
+      <c r="L990" s="15"/>
+      <c r="M990" s="15"/>
+      <c r="N990" s="15"/>
+      <c r="O990" s="15"/>
+      <c r="P990" s="15"/>
+      <c r="Q990" s="15"/>
+      <c r="R990" s="15"/>
+      <c r="S990" s="15"/>
+      <c r="T990" s="15"/>
+      <c r="U990" s="15"/>
+      <c r="V990" s="15"/>
+      <c r="W990" s="15"/>
+      <c r="X990" s="15"/>
+      <c r="Y990" s="15"/>
+      <c r="Z990" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -57274,10 +57314,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="53.375" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="15" width="13.5" customWidth="1"/>

</xml_diff>

<commit_message>
fix: reduce constraint message to (#413)
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="203">
   <si>
     <t>type</t>
   </si>
@@ -180,12 +180,6 @@
     <t>../person/language_preference</t>
   </si>
   <si>
-    <t>telegram_id</t>
-  </si>
-  <si>
-    <t>../person/telegram_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">true </t>
   </si>
   <si>
@@ -252,10 +246,28 @@
     <t>VMMC Client Age in Years</t>
   </si>
   <si>
-    <t>(.) &gt;= 18 and (.) &lt;= 75</t>
+    <t>(.) &gt;= 15 and (.) &lt;= 75</t>
   </si>
   <si>
-    <t>Client should be from 18 to 75 years old</t>
+    <t>Client should be from 15 to 75 years old</t>
+  </si>
+  <si>
+    <t>is_minor</t>
+  </si>
+  <si>
+    <t>${age_years} &lt; 18</t>
+  </si>
+  <si>
+    <t>select_one phone_owner</t>
+  </si>
+  <si>
+    <t>phone_owner</t>
+  </si>
+  <si>
+    <t>Whose Phone Number Is Minor Enrolling With?</t>
+  </si>
+  <si>
+    <t>${age_years} != ‘’</t>
   </si>
   <si>
     <t>Client Mobile phone number</t>
@@ -286,12 +298,6 @@
     <t>What is this client’s language of preference for the texts?</t>
   </si>
   <si>
-    <t>Telegram ID</t>
-  </si>
-  <si>
-    <t>This is for test purpose only</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -311,6 +317,18 @@
   </si>
   <si>
     <t>Ndebele</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>Minor’s</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>Guardian’s</t>
   </si>
   <si>
     <t>facilities</t>
@@ -638,7 +656,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Cambria"/>
     </font>
     <font>
@@ -655,7 +673,7 @@
     <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="11"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
@@ -680,7 +698,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -806,28 +824,28 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -836,19 +854,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -857,16 +875,16 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -888,8 +906,8 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ff2e75b6"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff843c0b"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffd0cece"/>
     </indexedColors>
   </colors>
@@ -1089,17 +1107,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1127,10 +1145,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1378,12 +1396,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1670,7 +1688,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1698,10 +1716,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1961,7 +1979,7 @@
     <col min="1" max="1" width="28.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="57" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.8516" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="43.1719" style="1" customWidth="1"/>
@@ -2669,12 +2687,8 @@
       <c r="Z19" s="6"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s" s="9">
-        <v>55</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -2683,9 +2697,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" t="s" s="9">
-        <v>56</v>
-      </c>
+      <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
@@ -2703,18 +2715,28 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="A21" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s" s="9">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s" s="9">
+        <v>40</v>
+      </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" t="s" s="9">
+        <v>17</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="L21" t="s" s="9">
+        <v>55</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -2735,14 +2757,14 @@
         <v>13</v>
       </c>
       <c r="B22" t="s" s="9">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s" s="9">
         <v>40</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" t="s" s="9">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2750,9 +2772,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" t="s" s="9">
-        <v>57</v>
-      </c>
+      <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -2770,10 +2790,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" t="s" s="9">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s" s="9">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s" s="9">
         <v>40</v>
@@ -2787,7 +2807,9 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="K23" t="s" s="9">
+        <v>56</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
@@ -2806,26 +2828,24 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" t="s" s="9">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s" s="9">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s" s="9">
         <v>40</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" t="s" s="9">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" t="s" s="9">
-        <v>58</v>
-      </c>
+      <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -2844,24 +2864,26 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" t="s" s="9">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s" s="9">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s" s="9">
         <v>40</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" t="s" s="9">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="K25" t="s" s="9">
+        <v>57</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -2880,26 +2902,18 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" t="s" s="9">
-        <v>42</v>
+        <v>41</v>
       </c>
-      <c r="B26" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s" s="9">
-        <v>40</v>
-      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" t="s" s="9">
-        <v>21</v>
-      </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" t="s" s="9">
-        <v>59</v>
-      </c>
+      <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -2948,18 +2962,26 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" t="s" s="9">
-        <v>41</v>
+        <v>42</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" t="s" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s" s="9">
+        <v>58</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="H28" t="s" s="9">
+        <v>46</v>
+      </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="K28" t="s" s="9">
+        <v>59</v>
+      </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
@@ -2976,28 +2998,30 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
+    <row r="29" ht="16" customHeight="1">
       <c r="A29" t="s" s="9">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s" s="9">
         <v>60</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="F29" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="G29" t="s" s="9">
+        <v>61</v>
+      </c>
       <c r="H29" t="s" s="9">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" t="s" s="9">
-        <v>61</v>
-      </c>
+      <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
@@ -3014,61 +3038,59 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" t="s" s="9">
-        <v>18</v>
+    <row r="30" ht="16" customHeight="1">
+      <c r="A30" t="s" s="10">
+        <v>13</v>
       </c>
-      <c r="B30" t="s" s="9">
-        <v>1</v>
+      <c r="B30" t="s" s="11">
+        <v>63</v>
       </c>
       <c r="C30" t="s" s="9">
-        <v>62</v>
+        <v>40</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" t="s" s="9">
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+    </row>
+    <row r="31" ht="16" customHeight="1">
+      <c r="A31" t="s" s="11">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s" s="11">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s" s="13">
+        <v>65</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" t="s" s="11">
+        <v>32</v>
+      </c>
+      <c r="F31" t="s" s="11">
         <v>33</v>
       </c>
-      <c r="G30" t="s" s="9">
-        <v>63</v>
-      </c>
-      <c r="H30" t="s" s="9">
-        <v>64</v>
-      </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s" s="11">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -3088,23 +3110,19 @@
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" ht="16" customHeight="1">
       <c r="A32" t="s" s="11">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s" s="11">
-        <v>30</v>
+        <v>1</v>
       </c>
-      <c r="C32" t="s" s="13">
-        <v>67</v>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" t="s" s="11">
+        <v>21</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" t="s" s="11">
-        <v>32</v>
-      </c>
-      <c r="F32" t="s" s="11">
-        <v>33</v>
-      </c>
+      <c r="F32" s="12"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="12"/>
@@ -3126,21 +3144,17 @@
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" t="s" s="11">
-        <v>18</v>
+    <row r="33" ht="16" customHeight="1">
+      <c r="A33" t="s" s="10">
+        <v>41</v>
       </c>
-      <c r="B33" t="s" s="11">
-        <v>1</v>
-      </c>
+      <c r="B33" s="12"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" t="s" s="11">
-        <v>21</v>
-      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -3160,56 +3174,68 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" t="s" s="10">
-        <v>41</v>
+    <row r="34" ht="16" customHeight="1">
+      <c r="A34" t="s" s="9">
+        <v>18</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+      <c r="B34" t="s" s="9">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s" s="9">
+        <v>67</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="H34" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+    </row>
+    <row r="35" ht="16" customHeight="1">
       <c r="A35" t="s" s="9">
         <v>18</v>
       </c>
       <c r="B35" t="s" s="9">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s" s="9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" t="s" s="9">
+        <v>71</v>
+      </c>
       <c r="F35" t="s" s="9">
         <v>33</v>
       </c>
       <c r="G35" t="s" s="9">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H35" t="s" s="9">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
@@ -3230,32 +3256,32 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" ht="16" customHeight="1">
       <c r="A36" t="s" s="9">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s" s="9">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s" s="9">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" t="s" s="9">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s" s="9">
         <v>33</v>
       </c>
       <c r="G36" t="s" s="9">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H36" t="s" s="9">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="K36" s="16"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -3272,32 +3298,26 @@
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" ht="16" customHeight="1">
       <c r="A37" t="s" s="9">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s" s="9">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s" s="9">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D37" s="6"/>
-      <c r="E37" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="F37" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="G37" t="s" s="9">
-        <v>79</v>
-      </c>
-      <c r="H37" t="s" s="9">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" t="s" s="9">
         <v>80</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
@@ -3314,30 +3334,24 @@
       <c r="Y37" s="6"/>
       <c r="Z37" s="6"/>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
+    <row r="38" ht="16" customHeight="1">
       <c r="A38" t="s" s="9">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s" s="9">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s" s="9">
-        <v>81</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="G38" t="s" s="9">
-        <v>82</v>
-      </c>
-      <c r="H38" t="s" s="9">
         <v>83</v>
       </c>
-      <c r="I38" t="s" s="16">
+      <c r="D38" t="s" s="9">
         <v>84</v>
       </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
@@ -3356,29 +3370,29 @@
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" ht="12.75" customHeight="1">
       <c r="A39" t="s" s="9">
         <v>18</v>
       </c>
       <c r="B39" t="s" s="9">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s" s="9">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="G39" t="s" s="9">
+        <v>86</v>
+      </c>
+      <c r="H39" t="s" s="9">
         <v>87</v>
       </c>
-      <c r="G39" t="s" s="9">
-        <v>82</v>
-      </c>
-      <c r="H39" t="s" s="9">
-        <v>83</v>
-      </c>
-      <c r="I39" t="s" s="16">
-        <v>84</v>
+      <c r="I39" t="s" s="17">
+        <v>88</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -3398,24 +3412,30 @@
       <c r="Y39" s="6"/>
       <c r="Z39" s="6"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="16" customHeight="1">
       <c r="A40" t="s" s="9">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s" s="9">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s" s="9">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" t="s" s="9">
-        <v>33</v>
+        <v>91</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="G40" t="s" s="9">
+        <v>86</v>
+      </c>
+      <c r="H40" t="s" s="9">
+        <v>87</v>
+      </c>
+      <c r="I40" t="s" s="17">
+        <v>88</v>
+      </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
@@ -3434,26 +3454,24 @@
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" ht="16" customHeight="1">
       <c r="A41" t="s" s="9">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s" s="9">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s" s="9">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" t="s" s="9">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
-      <c r="I41" t="s" s="9">
-        <v>91</v>
-      </c>
+      <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
@@ -3502,7 +3520,7 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" ht="16" customHeight="1">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -30561,23 +30579,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.6719" style="17" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="17.6719" style="17" customWidth="1"/>
-    <col min="4" max="6" width="13.5" style="17" customWidth="1"/>
-    <col min="7" max="26" width="8.5" style="17" customWidth="1"/>
-    <col min="27" max="16384" width="11.1719" style="17" customWidth="1"/>
+    <col min="1" max="1" width="19.6719" style="18" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="17.6719" style="18" customWidth="1"/>
+    <col min="4" max="6" width="13.5" style="18" customWidth="1"/>
+    <col min="7" max="26" width="8.5" style="18" customWidth="1"/>
+    <col min="27" max="16384" width="11.1719" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" ht="16" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s" s="11">
         <v>1</v>
@@ -30609,7 +30627,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" ht="16" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -30637,15 +30655,15 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" ht="16" customHeight="1">
       <c r="A3" t="s" s="11">
         <v>52</v>
       </c>
       <c r="B3" t="s" s="11">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s" s="11">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -30671,15 +30689,15 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="16" customHeight="1">
       <c r="A4" t="s" s="11">
         <v>52</v>
       </c>
       <c r="B4" t="s" s="11">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s" s="11">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -30705,15 +30723,15 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" ht="16" customHeight="1">
       <c r="A5" t="s" s="11">
         <v>52</v>
       </c>
       <c r="B5" t="s" s="11">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s" s="11">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -30739,7 +30757,7 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" ht="16" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -30767,15 +30785,15 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="18">
-        <v>99</v>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" t="s" s="11">
+        <v>82</v>
       </c>
-      <c r="B7" t="s" s="18">
-        <v>100</v>
+      <c r="B7" t="s" s="11">
+        <v>101</v>
       </c>
-      <c r="C7" t="s" s="18">
-        <v>101</v>
+      <c r="C7" t="s" s="11">
+        <v>102</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -30801,15 +30819,15 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="s" s="18">
-        <v>99</v>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" t="s" s="11">
+        <v>82</v>
       </c>
-      <c r="B8" t="s" s="18">
-        <v>102</v>
+      <c r="B8" t="s" s="11">
+        <v>103</v>
       </c>
-      <c r="C8" t="s" s="18">
-        <v>103</v>
+      <c r="C8" t="s" s="11">
+        <v>104</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -30835,16 +30853,10 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="s" s="18">
-        <v>99</v>
-      </c>
-      <c r="B9" t="s" s="18">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s" s="18">
-        <v>105</v>
-      </c>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -30869,14 +30881,14 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" t="s" s="18">
-        <v>99</v>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B10" t="s" s="18">
+      <c r="B10" t="s" s="19">
         <v>106</v>
       </c>
-      <c r="C10" t="s" s="18">
+      <c r="C10" t="s" s="19">
         <v>107</v>
       </c>
       <c r="D10" s="12"/>
@@ -30903,14 +30915,14 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="s" s="18">
-        <v>99</v>
+    <row r="11" ht="16" customHeight="1">
+      <c r="A11" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B11" t="s" s="18">
+      <c r="B11" t="s" s="19">
         <v>108</v>
       </c>
-      <c r="C11" t="s" s="18">
+      <c r="C11" t="s" s="19">
         <v>109</v>
       </c>
       <c r="D11" s="12"/>
@@ -30937,14 +30949,14 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" t="s" s="18">
-        <v>99</v>
+    <row r="12" ht="16" customHeight="1">
+      <c r="A12" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B12" t="s" s="18">
+      <c r="B12" t="s" s="19">
         <v>110</v>
       </c>
-      <c r="C12" t="s" s="18">
+      <c r="C12" t="s" s="19">
         <v>111</v>
       </c>
       <c r="D12" s="12"/>
@@ -30971,14 +30983,14 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" t="s" s="18">
-        <v>99</v>
+    <row r="13" ht="16" customHeight="1">
+      <c r="A13" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B13" t="s" s="18">
+      <c r="B13" t="s" s="19">
         <v>112</v>
       </c>
-      <c r="C13" t="s" s="18">
+      <c r="C13" t="s" s="19">
         <v>113</v>
       </c>
       <c r="D13" s="12"/>
@@ -31006,13 +31018,13 @@
       <c r="Z13" s="12"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" t="s" s="11">
-        <v>99</v>
+      <c r="A14" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" t="s" s="19">
         <v>114</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" t="s" s="19">
         <v>115</v>
       </c>
       <c r="D14" s="12"/>
@@ -31040,13 +31052,13 @@
       <c r="Z14" s="12"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" t="s" s="11">
-        <v>99</v>
+      <c r="A15" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B15" t="s" s="11">
+      <c r="B15" t="s" s="19">
         <v>116</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" t="s" s="19">
         <v>117</v>
       </c>
       <c r="D15" s="12"/>
@@ -31074,13 +31086,13 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="s" s="11">
-        <v>99</v>
+      <c r="A16" t="s" s="19">
+        <v>105</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" t="s" s="19">
         <v>118</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" t="s" s="19">
         <v>119</v>
       </c>
       <c r="D16" s="12"/>
@@ -31109,7 +31121,7 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s" s="11">
         <v>120</v>
@@ -31143,7 +31155,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>122</v>
@@ -31177,7 +31189,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>124</v>
@@ -31209,9 +31221,9 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s" s="11">
         <v>126</v>
@@ -31220,32 +31232,32 @@
         <v>127</v>
       </c>
       <c r="D20" s="12"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="19"/>
-    </row>
-    <row r="21" ht="15" customHeight="1">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>128</v>
@@ -31254,32 +31266,32 @@
         <v>129</v>
       </c>
       <c r="D21" s="12"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-    </row>
-    <row r="22" ht="15" customHeight="1">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>130</v>
@@ -31288,32 +31300,32 @@
         <v>131</v>
       </c>
       <c r="D22" s="12"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s" s="11">
         <v>132</v>
@@ -31322,32 +31334,32 @@
         <v>133</v>
       </c>
       <c r="D23" s="12"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s" s="11">
         <v>134</v>
@@ -31356,32 +31368,32 @@
         <v>135</v>
       </c>
       <c r="D24" s="12"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19"/>
-      <c r="X24" s="19"/>
-      <c r="Y24" s="19"/>
-      <c r="Z24" s="19"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s" s="11">
         <v>136</v>
@@ -31390,32 +31402,32 @@
         <v>137</v>
       </c>
       <c r="D25" s="12"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s" s="11">
         <v>138</v>
@@ -31424,32 +31436,32 @@
         <v>139</v>
       </c>
       <c r="D26" s="12"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="19"/>
-      <c r="X26" s="19"/>
-      <c r="Y26" s="19"/>
-      <c r="Z26" s="19"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+    </row>
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s" s="11">
         <v>140</v>
@@ -31458,32 +31470,32 @@
         <v>141</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+    </row>
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s" s="11">
         <v>142</v>
@@ -31492,32 +31504,32 @@
         <v>143</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+    </row>
+    <row r="29" ht="15" customHeight="1">
       <c r="A29" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s" s="11">
         <v>144</v>
@@ -31526,32 +31538,32 @@
         <v>145</v>
       </c>
       <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>146</v>
@@ -31564,7 +31576,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="I30" s="16"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
@@ -31585,7 +31597,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s" s="11">
         <v>148</v>
@@ -31598,7 +31610,7 @@
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
@@ -31619,7 +31631,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s" s="11">
         <v>150</v>
@@ -31653,7 +31665,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s" s="11">
         <v>152</v>
@@ -31687,7 +31699,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s" s="11">
         <v>154</v>
@@ -31700,7 +31712,7 @@
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="19"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -31721,7 +31733,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s" s="11">
         <v>156</v>
@@ -31734,7 +31746,7 @@
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="19"/>
+      <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
@@ -31755,7 +31767,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s" s="11">
         <v>158</v>
@@ -31768,7 +31780,7 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="19"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
@@ -31789,7 +31801,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s" s="11">
         <v>160</v>
@@ -31802,7 +31814,7 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="19"/>
+      <c r="I37" s="16"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
@@ -31823,7 +31835,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s" s="11">
         <v>162</v>
@@ -31836,7 +31848,7 @@
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="19"/>
+      <c r="I38" s="16"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
@@ -31857,7 +31869,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s" s="11">
         <v>164</v>
@@ -31870,7 +31882,7 @@
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="19"/>
+      <c r="I39" s="16"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
@@ -31891,7 +31903,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s" s="11">
         <v>166</v>
@@ -31904,7 +31916,7 @@
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="19"/>
+      <c r="I40" s="16"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
@@ -31925,7 +31937,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s" s="11">
         <v>168</v>
@@ -31938,7 +31950,7 @@
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="19"/>
+      <c r="I41" s="16"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
@@ -31959,7 +31971,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s" s="11">
         <v>170</v>
@@ -31972,7 +31984,7 @@
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="19"/>
+      <c r="I42" s="16"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
@@ -31993,7 +32005,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s" s="11">
         <v>172</v>
@@ -32006,7 +32018,7 @@
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="19"/>
+      <c r="I43" s="16"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
@@ -32027,7 +32039,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s" s="11">
         <v>174</v>
@@ -32040,7 +32052,7 @@
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="19"/>
+      <c r="I44" s="16"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
@@ -32061,7 +32073,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s" s="11">
         <v>176</v>
@@ -32074,7 +32086,7 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
+      <c r="I45" s="16"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
@@ -32095,7 +32107,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s" s="11">
         <v>178</v>
@@ -32108,7 +32120,7 @@
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
+      <c r="I46" s="16"/>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
@@ -32129,7 +32141,7 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s" s="11">
         <v>180</v>
@@ -32142,7 +32154,7 @@
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
+      <c r="I47" s="16"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
@@ -32163,7 +32175,7 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s" s="11">
         <v>182</v>
@@ -32197,7 +32209,7 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s" s="11">
         <v>184</v>
@@ -32231,7 +32243,7 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" t="s" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s" s="11">
         <v>186</v>
@@ -32264,9 +32276,15 @@
       <c r="Z50" s="12"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
+      <c r="A51" t="s" s="11">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s" s="11">
+        <v>188</v>
+      </c>
+      <c r="C51" t="s" s="11">
+        <v>189</v>
+      </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -32292,15 +32310,21 @@
       <c r="Z51" s="12"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
+      <c r="A52" t="s" s="11">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s" s="11">
+        <v>190</v>
+      </c>
+      <c r="C52" t="s" s="11">
+        <v>191</v>
+      </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="19"/>
+      <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
@@ -32320,9 +32344,15 @@
       <c r="Z52" s="12"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
+      <c r="A53" t="s" s="11">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s" s="11">
+        <v>192</v>
+      </c>
+      <c r="C53" t="s" s="11">
+        <v>193</v>
+      </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -32384,7 +32414,7 @@
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
@@ -57632,10 +57662,10 @@
       <c r="Z956" s="12"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="A957" s="19"/>
-      <c r="B957" s="19"/>
-      <c r="C957" s="19"/>
-      <c r="D957" s="19"/>
+      <c r="A957" s="12"/>
+      <c r="B957" s="12"/>
+      <c r="C957" s="12"/>
+      <c r="D957" s="12"/>
       <c r="E957" s="12"/>
       <c r="F957" s="12"/>
       <c r="G957" s="12"/>
@@ -57660,10 +57690,10 @@
       <c r="Z957" s="12"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="A958" s="19"/>
-      <c r="B958" s="19"/>
-      <c r="C958" s="19"/>
-      <c r="D958" s="19"/>
+      <c r="A958" s="12"/>
+      <c r="B958" s="12"/>
+      <c r="C958" s="12"/>
+      <c r="D958" s="12"/>
       <c r="E958" s="12"/>
       <c r="F958" s="12"/>
       <c r="G958" s="12"/>
@@ -57688,10 +57718,10 @@
       <c r="Z958" s="12"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="A959" s="19"/>
-      <c r="B959" s="19"/>
-      <c r="C959" s="19"/>
-      <c r="D959" s="19"/>
+      <c r="A959" s="12"/>
+      <c r="B959" s="12"/>
+      <c r="C959" s="12"/>
+      <c r="D959" s="12"/>
       <c r="E959" s="12"/>
       <c r="F959" s="12"/>
       <c r="G959" s="12"/>
@@ -57716,10 +57746,10 @@
       <c r="Z959" s="12"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="A960" s="19"/>
-      <c r="B960" s="19"/>
-      <c r="C960" s="19"/>
-      <c r="D960" s="19"/>
+      <c r="A960" s="16"/>
+      <c r="B960" s="16"/>
+      <c r="C960" s="16"/>
+      <c r="D960" s="16"/>
       <c r="E960" s="12"/>
       <c r="F960" s="12"/>
       <c r="G960" s="12"/>
@@ -57744,10 +57774,10 @@
       <c r="Z960" s="12"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="A961" s="19"/>
-      <c r="B961" s="19"/>
-      <c r="C961" s="19"/>
-      <c r="D961" s="19"/>
+      <c r="A961" s="16"/>
+      <c r="B961" s="16"/>
+      <c r="C961" s="16"/>
+      <c r="D961" s="16"/>
       <c r="E961" s="12"/>
       <c r="F961" s="12"/>
       <c r="G961" s="12"/>
@@ -57772,10 +57802,10 @@
       <c r="Z961" s="12"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="A962" s="19"/>
-      <c r="B962" s="19"/>
-      <c r="C962" s="19"/>
-      <c r="D962" s="19"/>
+      <c r="A962" s="16"/>
+      <c r="B962" s="16"/>
+      <c r="C962" s="16"/>
+      <c r="D962" s="16"/>
       <c r="E962" s="12"/>
       <c r="F962" s="12"/>
       <c r="G962" s="12"/>
@@ -57800,10 +57830,10 @@
       <c r="Z962" s="12"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="A963" s="19"/>
-      <c r="B963" s="19"/>
-      <c r="C963" s="19"/>
-      <c r="D963" s="19"/>
+      <c r="A963" s="16"/>
+      <c r="B963" s="16"/>
+      <c r="C963" s="16"/>
+      <c r="D963" s="16"/>
       <c r="E963" s="12"/>
       <c r="F963" s="12"/>
       <c r="G963" s="12"/>
@@ -57828,10 +57858,10 @@
       <c r="Z963" s="12"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="A964" s="19"/>
-      <c r="B964" s="19"/>
-      <c r="C964" s="19"/>
-      <c r="D964" s="19"/>
+      <c r="A964" s="16"/>
+      <c r="B964" s="16"/>
+      <c r="C964" s="16"/>
+      <c r="D964" s="16"/>
       <c r="E964" s="12"/>
       <c r="F964" s="12"/>
       <c r="G964" s="12"/>
@@ -57856,10 +57886,10 @@
       <c r="Z964" s="12"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="A965" s="19"/>
-      <c r="B965" s="19"/>
-      <c r="C965" s="19"/>
-      <c r="D965" s="19"/>
+      <c r="A965" s="16"/>
+      <c r="B965" s="16"/>
+      <c r="C965" s="16"/>
+      <c r="D965" s="16"/>
       <c r="E965" s="12"/>
       <c r="F965" s="12"/>
       <c r="G965" s="12"/>
@@ -57884,10 +57914,10 @@
       <c r="Z965" s="12"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="A966" s="19"/>
-      <c r="B966" s="19"/>
-      <c r="C966" s="19"/>
-      <c r="D966" s="19"/>
+      <c r="A966" s="16"/>
+      <c r="B966" s="16"/>
+      <c r="C966" s="16"/>
+      <c r="D966" s="16"/>
       <c r="E966" s="12"/>
       <c r="F966" s="12"/>
       <c r="G966" s="12"/>
@@ -57912,10 +57942,10 @@
       <c r="Z966" s="12"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="A967" s="19"/>
-      <c r="B967" s="19"/>
-      <c r="C967" s="19"/>
-      <c r="D967" s="19"/>
+      <c r="A967" s="16"/>
+      <c r="B967" s="16"/>
+      <c r="C967" s="16"/>
+      <c r="D967" s="16"/>
       <c r="E967" s="12"/>
       <c r="F967" s="12"/>
       <c r="G967" s="12"/>
@@ -57940,10 +57970,10 @@
       <c r="Z967" s="12"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="A968" s="19"/>
-      <c r="B968" s="19"/>
-      <c r="C968" s="19"/>
-      <c r="D968" s="19"/>
+      <c r="A968" s="16"/>
+      <c r="B968" s="16"/>
+      <c r="C968" s="16"/>
+      <c r="D968" s="16"/>
       <c r="E968" s="12"/>
       <c r="F968" s="12"/>
       <c r="G968" s="12"/>
@@ -57968,10 +57998,10 @@
       <c r="Z968" s="12"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="A969" s="19"/>
-      <c r="B969" s="19"/>
-      <c r="C969" s="19"/>
-      <c r="D969" s="19"/>
+      <c r="A969" s="16"/>
+      <c r="B969" s="16"/>
+      <c r="C969" s="16"/>
+      <c r="D969" s="16"/>
       <c r="E969" s="12"/>
       <c r="F969" s="12"/>
       <c r="G969" s="12"/>
@@ -57996,10 +58026,10 @@
       <c r="Z969" s="12"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="A970" s="19"/>
-      <c r="B970" s="19"/>
-      <c r="C970" s="19"/>
-      <c r="D970" s="19"/>
+      <c r="A970" s="16"/>
+      <c r="B970" s="16"/>
+      <c r="C970" s="16"/>
+      <c r="D970" s="16"/>
       <c r="E970" s="12"/>
       <c r="F970" s="12"/>
       <c r="G970" s="12"/>
@@ -58024,10 +58054,10 @@
       <c r="Z970" s="12"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="A971" s="19"/>
-      <c r="B971" s="19"/>
-      <c r="C971" s="19"/>
-      <c r="D971" s="19"/>
+      <c r="A971" s="16"/>
+      <c r="B971" s="16"/>
+      <c r="C971" s="16"/>
+      <c r="D971" s="16"/>
       <c r="E971" s="12"/>
       <c r="F971" s="12"/>
       <c r="G971" s="12"/>
@@ -58052,10 +58082,10 @@
       <c r="Z971" s="12"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="A972" s="19"/>
-      <c r="B972" s="19"/>
-      <c r="C972" s="19"/>
-      <c r="D972" s="19"/>
+      <c r="A972" s="16"/>
+      <c r="B972" s="16"/>
+      <c r="C972" s="16"/>
+      <c r="D972" s="16"/>
       <c r="E972" s="12"/>
       <c r="F972" s="12"/>
       <c r="G972" s="12"/>
@@ -58080,10 +58110,10 @@
       <c r="Z972" s="12"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="A973" s="19"/>
-      <c r="B973" s="19"/>
-      <c r="C973" s="19"/>
-      <c r="D973" s="19"/>
+      <c r="A973" s="16"/>
+      <c r="B973" s="16"/>
+      <c r="C973" s="16"/>
+      <c r="D973" s="16"/>
       <c r="E973" s="12"/>
       <c r="F973" s="12"/>
       <c r="G973" s="12"/>
@@ -58108,10 +58138,10 @@
       <c r="Z973" s="12"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="A974" s="19"/>
-      <c r="B974" s="19"/>
-      <c r="C974" s="19"/>
-      <c r="D974" s="19"/>
+      <c r="A974" s="16"/>
+      <c r="B974" s="16"/>
+      <c r="C974" s="16"/>
+      <c r="D974" s="16"/>
       <c r="E974" s="12"/>
       <c r="F974" s="12"/>
       <c r="G974" s="12"/>
@@ -58136,10 +58166,10 @@
       <c r="Z974" s="12"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="A975" s="19"/>
-      <c r="B975" s="19"/>
-      <c r="C975" s="19"/>
-      <c r="D975" s="19"/>
+      <c r="A975" s="16"/>
+      <c r="B975" s="16"/>
+      <c r="C975" s="16"/>
+      <c r="D975" s="16"/>
       <c r="E975" s="12"/>
       <c r="F975" s="12"/>
       <c r="G975" s="12"/>
@@ -58164,10 +58194,10 @@
       <c r="Z975" s="12"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="A976" s="19"/>
-      <c r="B976" s="19"/>
-      <c r="C976" s="19"/>
-      <c r="D976" s="19"/>
+      <c r="A976" s="16"/>
+      <c r="B976" s="16"/>
+      <c r="C976" s="16"/>
+      <c r="D976" s="16"/>
       <c r="E976" s="12"/>
       <c r="F976" s="12"/>
       <c r="G976" s="12"/>
@@ -58192,10 +58222,10 @@
       <c r="Z976" s="12"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="A977" s="19"/>
-      <c r="B977" s="19"/>
-      <c r="C977" s="19"/>
-      <c r="D977" s="19"/>
+      <c r="A977" s="16"/>
+      <c r="B977" s="16"/>
+      <c r="C977" s="16"/>
+      <c r="D977" s="16"/>
       <c r="E977" s="12"/>
       <c r="F977" s="12"/>
       <c r="G977" s="12"/>
@@ -58220,10 +58250,10 @@
       <c r="Z977" s="12"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="A978" s="19"/>
-      <c r="B978" s="19"/>
-      <c r="C978" s="19"/>
-      <c r="D978" s="19"/>
+      <c r="A978" s="16"/>
+      <c r="B978" s="16"/>
+      <c r="C978" s="16"/>
+      <c r="D978" s="16"/>
       <c r="E978" s="12"/>
       <c r="F978" s="12"/>
       <c r="G978" s="12"/>
@@ -58248,10 +58278,10 @@
       <c r="Z978" s="12"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="A979" s="19"/>
-      <c r="B979" s="19"/>
-      <c r="C979" s="19"/>
-      <c r="D979" s="19"/>
+      <c r="A979" s="16"/>
+      <c r="B979" s="16"/>
+      <c r="C979" s="16"/>
+      <c r="D979" s="16"/>
       <c r="E979" s="12"/>
       <c r="F979" s="12"/>
       <c r="G979" s="12"/>
@@ -58276,10 +58306,10 @@
       <c r="Z979" s="12"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="A980" s="19"/>
-      <c r="B980" s="19"/>
-      <c r="C980" s="19"/>
-      <c r="D980" s="19"/>
+      <c r="A980" s="16"/>
+      <c r="B980" s="16"/>
+      <c r="C980" s="16"/>
+      <c r="D980" s="16"/>
       <c r="E980" s="12"/>
       <c r="F980" s="12"/>
       <c r="G980" s="12"/>
@@ -58304,10 +58334,10 @@
       <c r="Z980" s="12"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="A981" s="19"/>
-      <c r="B981" s="19"/>
-      <c r="C981" s="19"/>
-      <c r="D981" s="19"/>
+      <c r="A981" s="16"/>
+      <c r="B981" s="16"/>
+      <c r="C981" s="16"/>
+      <c r="D981" s="16"/>
       <c r="E981" s="12"/>
       <c r="F981" s="12"/>
       <c r="G981" s="12"/>
@@ -58332,10 +58362,10 @@
       <c r="Z981" s="12"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="A982" s="19"/>
-      <c r="B982" s="19"/>
-      <c r="C982" s="19"/>
-      <c r="D982" s="19"/>
+      <c r="A982" s="16"/>
+      <c r="B982" s="16"/>
+      <c r="C982" s="16"/>
+      <c r="D982" s="16"/>
       <c r="E982" s="12"/>
       <c r="F982" s="12"/>
       <c r="G982" s="12"/>
@@ -58360,10 +58390,10 @@
       <c r="Z982" s="12"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="A983" s="19"/>
-      <c r="B983" s="19"/>
-      <c r="C983" s="19"/>
-      <c r="D983" s="19"/>
+      <c r="A983" s="16"/>
+      <c r="B983" s="16"/>
+      <c r="C983" s="16"/>
+      <c r="D983" s="16"/>
       <c r="E983" s="12"/>
       <c r="F983" s="12"/>
       <c r="G983" s="12"/>
@@ -58388,10 +58418,10 @@
       <c r="Z983" s="12"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="A984" s="19"/>
-      <c r="B984" s="19"/>
-      <c r="C984" s="19"/>
-      <c r="D984" s="19"/>
+      <c r="A984" s="16"/>
+      <c r="B984" s="16"/>
+      <c r="C984" s="16"/>
+      <c r="D984" s="16"/>
       <c r="E984" s="12"/>
       <c r="F984" s="12"/>
       <c r="G984" s="12"/>
@@ -58416,10 +58446,10 @@
       <c r="Z984" s="12"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="A985" s="19"/>
-      <c r="B985" s="19"/>
-      <c r="C985" s="19"/>
-      <c r="D985" s="19"/>
+      <c r="A985" s="16"/>
+      <c r="B985" s="16"/>
+      <c r="C985" s="16"/>
+      <c r="D985" s="16"/>
       <c r="E985" s="12"/>
       <c r="F985" s="12"/>
       <c r="G985" s="12"/>
@@ -58444,10 +58474,10 @@
       <c r="Z985" s="12"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="A986" s="19"/>
-      <c r="B986" s="19"/>
-      <c r="C986" s="19"/>
-      <c r="D986" s="19"/>
+      <c r="A986" s="16"/>
+      <c r="B986" s="16"/>
+      <c r="C986" s="16"/>
+      <c r="D986" s="16"/>
       <c r="E986" s="12"/>
       <c r="F986" s="12"/>
       <c r="G986" s="12"/>
@@ -58472,10 +58502,10 @@
       <c r="Z986" s="12"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="A987" s="19"/>
-      <c r="B987" s="19"/>
-      <c r="C987" s="19"/>
-      <c r="D987" s="19"/>
+      <c r="A987" s="16"/>
+      <c r="B987" s="16"/>
+      <c r="C987" s="16"/>
+      <c r="D987" s="16"/>
       <c r="E987" s="12"/>
       <c r="F987" s="12"/>
       <c r="G987" s="12"/>
@@ -58500,10 +58530,10 @@
       <c r="Z987" s="12"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="A988" s="19"/>
-      <c r="B988" s="19"/>
-      <c r="C988" s="19"/>
-      <c r="D988" s="19"/>
+      <c r="A988" s="16"/>
+      <c r="B988" s="16"/>
+      <c r="C988" s="16"/>
+      <c r="D988" s="16"/>
       <c r="E988" s="12"/>
       <c r="F988" s="12"/>
       <c r="G988" s="12"/>
@@ -58528,10 +58558,10 @@
       <c r="Z988" s="12"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="A989" s="19"/>
-      <c r="B989" s="19"/>
-      <c r="C989" s="19"/>
-      <c r="D989" s="19"/>
+      <c r="A989" s="16"/>
+      <c r="B989" s="16"/>
+      <c r="C989" s="16"/>
+      <c r="D989" s="16"/>
       <c r="E989" s="12"/>
       <c r="F989" s="12"/>
       <c r="G989" s="12"/>
@@ -58556,10 +58586,10 @@
       <c r="Z989" s="12"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="A990" s="19"/>
-      <c r="B990" s="19"/>
-      <c r="C990" s="19"/>
-      <c r="D990" s="19"/>
+      <c r="A990" s="16"/>
+      <c r="B990" s="16"/>
+      <c r="C990" s="16"/>
+      <c r="D990" s="16"/>
       <c r="E990" s="12"/>
       <c r="F990" s="12"/>
       <c r="G990" s="12"/>
@@ -58582,6 +58612,90 @@
       <c r="X990" s="12"/>
       <c r="Y990" s="12"/>
       <c r="Z990" s="12"/>
+    </row>
+    <row r="991" ht="15.75" customHeight="1">
+      <c r="A991" s="16"/>
+      <c r="B991" s="16"/>
+      <c r="C991" s="16"/>
+      <c r="D991" s="16"/>
+      <c r="E991" s="12"/>
+      <c r="F991" s="12"/>
+      <c r="G991" s="12"/>
+      <c r="H991" s="12"/>
+      <c r="I991" s="12"/>
+      <c r="J991" s="12"/>
+      <c r="K991" s="12"/>
+      <c r="L991" s="12"/>
+      <c r="M991" s="12"/>
+      <c r="N991" s="12"/>
+      <c r="O991" s="12"/>
+      <c r="P991" s="12"/>
+      <c r="Q991" s="12"/>
+      <c r="R991" s="12"/>
+      <c r="S991" s="12"/>
+      <c r="T991" s="12"/>
+      <c r="U991" s="12"/>
+      <c r="V991" s="12"/>
+      <c r="W991" s="12"/>
+      <c r="X991" s="12"/>
+      <c r="Y991" s="12"/>
+      <c r="Z991" s="12"/>
+    </row>
+    <row r="992" ht="15.75" customHeight="1">
+      <c r="A992" s="16"/>
+      <c r="B992" s="16"/>
+      <c r="C992" s="16"/>
+      <c r="D992" s="16"/>
+      <c r="E992" s="12"/>
+      <c r="F992" s="12"/>
+      <c r="G992" s="12"/>
+      <c r="H992" s="12"/>
+      <c r="I992" s="12"/>
+      <c r="J992" s="12"/>
+      <c r="K992" s="12"/>
+      <c r="L992" s="12"/>
+      <c r="M992" s="12"/>
+      <c r="N992" s="12"/>
+      <c r="O992" s="12"/>
+      <c r="P992" s="12"/>
+      <c r="Q992" s="12"/>
+      <c r="R992" s="12"/>
+      <c r="S992" s="12"/>
+      <c r="T992" s="12"/>
+      <c r="U992" s="12"/>
+      <c r="V992" s="12"/>
+      <c r="W992" s="12"/>
+      <c r="X992" s="12"/>
+      <c r="Y992" s="12"/>
+      <c r="Z992" s="12"/>
+    </row>
+    <row r="993" ht="15.75" customHeight="1">
+      <c r="A993" s="16"/>
+      <c r="B993" s="16"/>
+      <c r="C993" s="16"/>
+      <c r="D993" s="16"/>
+      <c r="E993" s="12"/>
+      <c r="F993" s="12"/>
+      <c r="G993" s="12"/>
+      <c r="H993" s="12"/>
+      <c r="I993" s="12"/>
+      <c r="J993" s="12"/>
+      <c r="K993" s="12"/>
+      <c r="L993" s="12"/>
+      <c r="M993" s="12"/>
+      <c r="N993" s="12"/>
+      <c r="O993" s="12"/>
+      <c r="P993" s="12"/>
+      <c r="Q993" s="12"/>
+      <c r="R993" s="12"/>
+      <c r="S993" s="12"/>
+      <c r="T993" s="12"/>
+      <c r="U993" s="12"/>
+      <c r="V993" s="12"/>
+      <c r="W993" s="12"/>
+      <c r="X993" s="12"/>
+      <c r="Y993" s="12"/>
+      <c r="Z993" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
@@ -58610,19 +58724,19 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="21">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s" s="21">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C1" t="s" s="21">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s" s="21">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E1" t="s" s="21">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -58637,19 +58751,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="22">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s" s="23">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C2" s="24">
         <v>43900</v>
       </c>
       <c r="D2" t="s" s="23">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s" s="23">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -58663,140 +58777,140 @@
       <c r="O2" s="25"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>

</xml_diff>

<commit_message>
fix: showing phone ower field for non minors (#415)
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/enroll.xlsx
+++ b/zazic-scale-up/forms/app/enroll.xlsx
@@ -255,7 +255,7 @@
     <t>is_minor</t>
   </si>
   <si>
-    <t>${age_years} &lt; 18</t>
+    <t>(${age_years}) &gt;= 15 and (${age_years}) &lt;= 17</t>
   </si>
   <si>
     <t>select_one phone_owner</t>
@@ -267,7 +267,7 @@
     <t>Whose Phone Number Is Minor Enrolling With?</t>
   </si>
   <si>
-    <t>${age_years} != ‘’</t>
+    <t>${is_minor} = ‘true’</t>
   </si>
   <si>
     <t>Client Mobile phone number</t>
@@ -1986,7 +1986,7 @@
     <col min="8" max="8" width="50.1719" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.1719" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7812" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.3516" style="1" customWidth="1"/>
     <col min="14" max="16" width="13.5" style="1" customWidth="1"/>

</xml_diff>